<commit_message>
essaie de changer le logo d'equipe + modification dans la revue de code
</commit_message>
<xml_diff>
--- a/Fichiers equipe/revue_code_Elie.xlsx
+++ b/Fichiers equipe/revue_code_Elie.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\efrie\OneDrive - Collège de Bois-de-Boulogne\genie logiciel\Session 5 - Automne 2023\Maintenance logiciel\5GP-Travail_pratique_1\Fichiers equipe\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4839B378-3EC9-4B2C-8BBE-CB83E4EC32B0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A579B386-7938-481E-92D1-B82628FB6C38}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{A048998D-8A6E-437B-863F-D5E4D7A0533E}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="36">
   <si>
     <t>FICHE DE REVUE DE CODE</t>
   </si>
@@ -123,6 +123,27 @@
   </si>
   <si>
     <t>La variable (TEMPS_EPREUVE) n'a jamais été déclarée ou initialisée</t>
+  </si>
+  <si>
+    <t>Défaut+ Cosmétique</t>
+  </si>
+  <si>
+    <t>Les retours à la ligne ne sont pas respecter selon PEP8 (les espcae entre les fonctions et methodes )</t>
+  </si>
+  <si>
+    <t>Partout</t>
+  </si>
+  <si>
+    <t>les noms des fonctions  (splacher et splasher)</t>
+  </si>
+  <si>
+    <t>43+48+104</t>
+  </si>
+  <si>
+    <t>défaut</t>
+  </si>
+  <si>
+    <t>Toutes les fonctions sont appellés dans programme-principal</t>
   </si>
 </sst>
 </file>
@@ -557,8 +578,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{61EF6733-6B20-4ADE-95E8-4F31CB65AA28}">
   <dimension ref="A1:G36"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="D17" sqref="D17"/>
+    <sheetView tabSelected="1" topLeftCell="A10" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="D30" sqref="D30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -724,13 +745,19 @@
       </c>
       <c r="G14" s="4"/>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="4">
         <v>4</v>
       </c>
-      <c r="B15" s="4"/>
-      <c r="C15" s="4"/>
-      <c r="D15" s="7"/>
+      <c r="B15" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="C15" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="D15" s="7" t="s">
+        <v>30</v>
+      </c>
       <c r="E15" s="4"/>
       <c r="F15" s="4" t="s">
         <v>7</v>
@@ -739,11 +766,17 @@
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A16" s="4">
-        <v>6</v>
-      </c>
-      <c r="B16" s="4"/>
-      <c r="C16" s="4"/>
-      <c r="D16" s="7"/>
+        <v>5</v>
+      </c>
+      <c r="B16" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="C16" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="D16" s="7" t="s">
+        <v>32</v>
+      </c>
       <c r="E16" s="4"/>
       <c r="F16" s="4" t="s">
         <v>7</v>
@@ -752,11 +785,17 @@
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A17" s="4">
-        <v>7</v>
-      </c>
-      <c r="B17" s="4"/>
-      <c r="C17" s="4"/>
-      <c r="D17" s="7"/>
+        <v>6</v>
+      </c>
+      <c r="B17" s="4">
+        <v>128</v>
+      </c>
+      <c r="C17" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="D17" s="7" t="s">
+        <v>35</v>
+      </c>
       <c r="E17" s="4"/>
       <c r="F17" s="4" t="s">
         <v>7</v>
@@ -765,7 +804,7 @@
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A18" s="4">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B18" s="4"/>
       <c r="C18" s="4"/>
@@ -778,7 +817,7 @@
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A19" s="4">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B19" s="4"/>
       <c r="C19" s="4"/>
@@ -791,7 +830,7 @@
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A20" s="4">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B20" s="4"/>
       <c r="C20" s="4"/>
@@ -804,7 +843,7 @@
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A21" s="4">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B21" s="4"/>
       <c r="C21" s="4"/>
@@ -817,7 +856,7 @@
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A22" s="4">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B22" s="4"/>
       <c r="C22" s="4"/>
@@ -828,7 +867,7 @@
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A23" s="4">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B23" s="4"/>
       <c r="C23" s="4"/>
@@ -839,7 +878,7 @@
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A24" s="4">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B24" s="4"/>
       <c r="C24" s="4"/>
@@ -850,7 +889,7 @@
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A25" s="4">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B25" s="4"/>
       <c r="C25" s="4"/>
@@ -861,7 +900,7 @@
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A26" s="4">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B26" s="4"/>
       <c r="C26" s="4"/>
@@ -872,7 +911,7 @@
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A27" s="4">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B27" s="4"/>
       <c r="C27" s="4"/>
@@ -883,7 +922,7 @@
     </row>
     <row r="28" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A28" s="4">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B28" s="4"/>
       <c r="C28" s="4"/>
@@ -894,7 +933,7 @@
     </row>
     <row r="29" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A29" s="4">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B29" s="4"/>
       <c r="C29" s="4"/>
@@ -905,7 +944,7 @@
     </row>
     <row r="30" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A30" s="4">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B30" s="4"/>
       <c r="C30" s="4"/>
@@ -916,7 +955,7 @@
     </row>
     <row r="31" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A31" s="4">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B31" s="4"/>
       <c r="C31" s="4"/>
@@ -927,7 +966,7 @@
     </row>
     <row r="32" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A32" s="4">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B32" s="4"/>
       <c r="C32" s="4"/>
@@ -938,7 +977,7 @@
     </row>
     <row r="33" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A33" s="4">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B33" s="4"/>
       <c r="C33" s="4"/>
@@ -949,7 +988,7 @@
     </row>
     <row r="34" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A34" s="4">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B34" s="4"/>
       <c r="C34" s="4"/>
@@ -960,7 +999,7 @@
     </row>
     <row r="35" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A35" s="4">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B35" s="4"/>
       <c r="C35" s="4"/>
@@ -971,7 +1010,7 @@
     </row>
     <row r="36" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A36" s="4">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B36" s="4"/>
       <c r="C36" s="4"/>

</xml_diff>

<commit_message>
modification de revue de code Elie
</commit_message>
<xml_diff>
--- a/Fichiers equipe/revue_code_Elie.xlsx
+++ b/Fichiers equipe/revue_code_Elie.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\efrie\OneDrive - Collège de Bois-de-Boulogne\genie logiciel\Session 5 - Automne 2023\Maintenance logiciel\5GP-Travail_pratique_1\Fichiers equipe\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lion0203\projets\5GP-Travail_pratique_1\Fichiers equipe\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A579B386-7938-481E-92D1-B82628FB6C38}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EC5D5221-42F8-4279-BBA0-F8836466A87C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{A048998D-8A6E-437B-863F-D5E4D7A0533E}"/>
+    <workbookView xWindow="38280" yWindow="5355" windowWidth="38640" windowHeight="15720" xr2:uid="{A048998D-8A6E-437B-863F-D5E4D7A0533E}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="77" uniqueCount="45">
   <si>
     <t>FICHE DE REVUE DE CODE</t>
   </si>
@@ -107,50 +107,221 @@
     <t>Amélioration</t>
   </si>
   <si>
-    <t>Il n'ya pas de main dans l'application</t>
-  </si>
-  <si>
     <t>Cosmétique</t>
   </si>
   <si>
     <t>44-50-57-59 etc</t>
   </si>
   <si>
-    <t>Des lignes trop longues dépassant 80 caractères.</t>
-  </si>
-  <si>
     <t>Erreur</t>
   </si>
   <si>
-    <t>La variable (TEMPS_EPREUVE) n'a jamais été déclarée ou initialisée</t>
-  </si>
-  <si>
     <t>Défaut+ Cosmétique</t>
   </si>
   <si>
-    <t>Les retours à la ligne ne sont pas respecter selon PEP8 (les espcae entre les fonctions et methodes )</t>
-  </si>
-  <si>
     <t>Partout</t>
   </si>
   <si>
-    <t>les noms des fonctions  (splacher et splasher)</t>
-  </si>
-  <si>
     <t>43+48+104</t>
   </si>
   <si>
-    <t>défaut</t>
-  </si>
-  <si>
-    <t>Toutes les fonctions sont appellés dans programme-principal</t>
+    <t>en cours</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Amélioration +Cosmétique </t>
+  </si>
+  <si>
+    <t>Défaut</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Il n'ya pas de main dans l'application </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>(monsieur_tartempion.py)</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>Des lignes trop longues dépassant 80 caractères.</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>(monsieur_tartempion.py)</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>La variable (TEMPS_EPREUVE) n'a jamais été déclarée ou initialisée</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>(monsieur_tartempion.py)</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>Les retours à la ligne ne sont pas respecter selon PEP8 (les espcae entre les fonctions et methodes)</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>(monsieur_tartempion.py)</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">les noms des fonctions  (splacher et splasher) </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> (monsieur_tartempion.py)</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Toutes les fonctions sont appellés dans programme-principal </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>(monsieur_tartempion.py)</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>une partie du code qui est mit en commentaire</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> (monsieur_tartempion.py)</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>Laisser une ligne vide à la fin du code</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> (monsieur_tartempion.py)</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Manque de commentaire dans le code </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> (monsieur_tartempion.py)</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>Lignes vierges ne sont pas toujours respectés entre les partie du code pour la lisibilité</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> (monsieur_tartempion.py)</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Noms de variables non significatifs  (ex: banque, k) </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>(monsieur_tartempion.py)</t>
+    </r>
+  </si>
+  <si>
+    <t>Défaut + Erreur</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">La variablle (temps_actuel) est utilisé avant de l'assigner une valeurs </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> (monsieur_tartempion.py)</t>
+    </r>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -178,6 +349,13 @@
       <b/>
       <sz val="14"/>
       <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -236,7 +414,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
@@ -253,14 +431,23 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -280,7 +467,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Thème Office">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -578,31 +765,31 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{61EF6733-6B20-4ADE-95E8-4F31CB65AA28}">
   <dimension ref="A1:G36"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="D30" sqref="D30"/>
+    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="K10" sqref="K10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="6" customWidth="1"/>
     <col min="2" max="2" width="14.42578125" customWidth="1"/>
-    <col min="3" max="3" width="18.7109375" customWidth="1"/>
-    <col min="4" max="4" width="90.7109375" customWidth="1"/>
+    <col min="3" max="3" width="25.7109375" customWidth="1"/>
+    <col min="4" max="4" width="95.7109375" customWidth="1"/>
     <col min="5" max="5" width="17" customWidth="1"/>
     <col min="6" max="6" width="20.28515625" customWidth="1"/>
     <col min="7" max="7" width="14.28515625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A1" s="10" t="s">
+      <c r="A1" s="9" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="10"/>
-      <c r="C1" s="10"/>
-      <c r="D1" s="10"/>
-      <c r="E1" s="10"/>
-      <c r="F1" s="10"/>
-      <c r="G1" s="10"/>
+      <c r="B1" s="9"/>
+      <c r="C1" s="9"/>
+      <c r="D1" s="9"/>
+      <c r="E1" s="9"/>
+      <c r="F1" s="9"/>
+      <c r="G1" s="9"/>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="C3" t="s">
@@ -694,187 +881,253 @@
       <c r="A12" s="4">
         <v>1</v>
       </c>
-      <c r="B12" s="9"/>
-      <c r="C12" s="4" t="s">
+      <c r="B12" s="12" t="s">
+        <v>27</v>
+      </c>
+      <c r="C12" s="13" t="s">
         <v>22</v>
       </c>
-      <c r="D12" s="4" t="s">
-        <v>23</v>
-      </c>
-      <c r="E12" s="4"/>
-      <c r="F12" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="G12" s="4"/>
+      <c r="D12" s="13" t="s">
+        <v>32</v>
+      </c>
+      <c r="E12" s="13"/>
+      <c r="F12" s="13" t="s">
+        <v>7</v>
+      </c>
+      <c r="G12" s="13" t="s">
+        <v>29</v>
+      </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A13" s="4">
         <v>2</v>
       </c>
-      <c r="B13" s="8" t="s">
-        <v>25</v>
-      </c>
-      <c r="C13" s="4" t="s">
+      <c r="B13" s="13" t="s">
         <v>24</v>
       </c>
-      <c r="D13" s="7" t="s">
-        <v>26</v>
-      </c>
-      <c r="E13" s="4"/>
-      <c r="F13" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="G13" s="4"/>
+      <c r="C13" s="13" t="s">
+        <v>23</v>
+      </c>
+      <c r="D13" s="10" t="s">
+        <v>33</v>
+      </c>
+      <c r="E13" s="13"/>
+      <c r="F13" s="13" t="s">
+        <v>7</v>
+      </c>
+      <c r="G13" s="13" t="s">
+        <v>29</v>
+      </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A14" s="4">
         <v>3</v>
       </c>
-      <c r="B14" s="4">
+      <c r="B14" s="13">
         <v>205</v>
       </c>
-      <c r="C14" s="4" t="s">
+      <c r="C14" s="13" t="s">
+        <v>25</v>
+      </c>
+      <c r="D14" s="10" t="s">
+        <v>34</v>
+      </c>
+      <c r="E14" s="13"/>
+      <c r="F14" s="13" t="s">
+        <v>7</v>
+      </c>
+      <c r="G14" s="13" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" ht="39.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A15" s="10">
+        <v>4</v>
+      </c>
+      <c r="B15" s="11" t="s">
         <v>27</v>
       </c>
-      <c r="D14" s="7" t="s">
-        <v>28</v>
-      </c>
-      <c r="E14" s="4"/>
-      <c r="F14" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="G14" s="4"/>
-    </row>
-    <row r="15" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="4">
-        <v>4</v>
-      </c>
-      <c r="B15" s="4" t="s">
-        <v>31</v>
-      </c>
-      <c r="C15" s="4" t="s">
+      <c r="C15" s="10" t="s">
+        <v>26</v>
+      </c>
+      <c r="D15" s="10" t="s">
+        <v>35</v>
+      </c>
+      <c r="E15" s="10"/>
+      <c r="F15" s="10" t="s">
+        <v>7</v>
+      </c>
+      <c r="G15" s="10" t="s">
         <v>29</v>
       </c>
-      <c r="D15" s="7" t="s">
-        <v>30</v>
-      </c>
-      <c r="E15" s="4"/>
-      <c r="F15" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="G15" s="4"/>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A16" s="4">
         <v>5</v>
       </c>
-      <c r="B16" s="4" t="s">
-        <v>33</v>
-      </c>
-      <c r="C16" s="4" t="s">
+      <c r="B16" s="13" t="s">
+        <v>28</v>
+      </c>
+      <c r="C16" s="13" t="s">
+        <v>26</v>
+      </c>
+      <c r="D16" s="10" t="s">
+        <v>36</v>
+      </c>
+      <c r="E16" s="13"/>
+      <c r="F16" s="13" t="s">
+        <v>7</v>
+      </c>
+      <c r="G16" s="13" t="s">
         <v>29</v>
       </c>
-      <c r="D16" s="7" t="s">
-        <v>32</v>
-      </c>
-      <c r="E16" s="4"/>
-      <c r="F16" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="G16" s="4"/>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A17" s="4">
         <v>6</v>
       </c>
-      <c r="B17" s="4">
+      <c r="B17" s="13">
         <v>128</v>
       </c>
-      <c r="C17" s="4" t="s">
-        <v>34</v>
-      </c>
-      <c r="D17" s="7" t="s">
-        <v>35</v>
-      </c>
-      <c r="E17" s="4"/>
-      <c r="F17" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="G17" s="4"/>
+      <c r="C17" s="13" t="s">
+        <v>31</v>
+      </c>
+      <c r="D17" s="10" t="s">
+        <v>37</v>
+      </c>
+      <c r="E17" s="13"/>
+      <c r="F17" s="13" t="s">
+        <v>7</v>
+      </c>
+      <c r="G17" s="13" t="s">
+        <v>29</v>
+      </c>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A18" s="4">
         <v>7</v>
       </c>
-      <c r="B18" s="4"/>
-      <c r="C18" s="4"/>
-      <c r="D18" s="7"/>
-      <c r="E18" s="4"/>
-      <c r="F18" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="G18" s="4"/>
-    </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B18" s="13">
+        <v>54</v>
+      </c>
+      <c r="C18" s="13" t="s">
+        <v>23</v>
+      </c>
+      <c r="D18" s="10" t="s">
+        <v>38</v>
+      </c>
+      <c r="E18" s="13"/>
+      <c r="F18" s="13" t="s">
+        <v>7</v>
+      </c>
+      <c r="G18" s="13" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" ht="39.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="4">
         <v>8</v>
       </c>
-      <c r="B19" s="4"/>
-      <c r="C19" s="4"/>
-      <c r="D19" s="4"/>
-      <c r="E19" s="4"/>
-      <c r="F19" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="G19" s="4"/>
+      <c r="B19" s="12" t="s">
+        <v>27</v>
+      </c>
+      <c r="C19" s="13" t="s">
+        <v>30</v>
+      </c>
+      <c r="D19" s="13" t="s">
+        <v>41</v>
+      </c>
+      <c r="E19" s="13"/>
+      <c r="F19" s="13" t="s">
+        <v>7</v>
+      </c>
+      <c r="G19" s="13" t="s">
+        <v>29</v>
+      </c>
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A20" s="4">
         <v>9</v>
       </c>
-      <c r="B20" s="4"/>
-      <c r="C20" s="4"/>
-      <c r="D20" s="4"/>
-      <c r="E20" s="4"/>
-      <c r="F20" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="G20" s="4"/>
+      <c r="B20" s="13">
+        <v>241</v>
+      </c>
+      <c r="C20" s="13" t="s">
+        <v>22</v>
+      </c>
+      <c r="D20" s="13" t="s">
+        <v>39</v>
+      </c>
+      <c r="E20" s="13"/>
+      <c r="F20" s="13" t="s">
+        <v>7</v>
+      </c>
+      <c r="G20" s="13" t="s">
+        <v>29</v>
+      </c>
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A21" s="4">
         <v>10</v>
       </c>
-      <c r="B21" s="4"/>
-      <c r="C21" s="4"/>
-      <c r="D21" s="7"/>
-      <c r="E21" s="4"/>
-      <c r="F21" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="G21" s="4"/>
+      <c r="B21" s="12" t="s">
+        <v>27</v>
+      </c>
+      <c r="C21" s="13" t="s">
+        <v>31</v>
+      </c>
+      <c r="D21" s="10" t="s">
+        <v>40</v>
+      </c>
+      <c r="E21" s="13"/>
+      <c r="F21" s="13" t="s">
+        <v>7</v>
+      </c>
+      <c r="G21" s="13" t="s">
+        <v>29</v>
+      </c>
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A22" s="4">
         <v>11</v>
       </c>
-      <c r="B22" s="4"/>
-      <c r="C22" s="4"/>
-      <c r="D22" s="7"/>
+      <c r="B22" s="8" t="s">
+        <v>27</v>
+      </c>
+      <c r="C22" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="D22" s="7" t="s">
+        <v>42</v>
+      </c>
       <c r="E22" s="4"/>
-      <c r="F22" s="4"/>
-      <c r="G22" s="4"/>
+      <c r="F22" s="13" t="s">
+        <v>7</v>
+      </c>
+      <c r="G22" s="13" t="s">
+        <v>29</v>
+      </c>
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A23" s="4">
         <v>12</v>
       </c>
-      <c r="B23" s="4"/>
-      <c r="C23" s="4"/>
-      <c r="D23" s="7"/>
+      <c r="B23" s="4">
+        <v>162</v>
+      </c>
+      <c r="C23" s="4" t="s">
+        <v>43</v>
+      </c>
+      <c r="D23" s="7" t="s">
+        <v>44</v>
+      </c>
       <c r="E23" s="4"/>
-      <c r="F23" s="4"/>
-      <c r="G23" s="4"/>
+      <c r="F23" s="13" t="s">
+        <v>7</v>
+      </c>
+      <c r="G23" s="13" t="s">
+        <v>29</v>
+      </c>
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A24" s="4">

</xml_diff>

<commit_message>
modification dans le revu de code
</commit_message>
<xml_diff>
--- a/Fichiers equipe/revue_code_Elie.xlsx
+++ b/Fichiers equipe/revue_code_Elie.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\efrie\OneDrive - Collège de Bois-de-Boulogne\genie logiciel\Session 5 - Automne 2023\Maintenance logiciel\5GP-Travail_pratique_1\Fichiers equipe\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lion0203\projets\5GP-Travail_pratique_1\Fichiers equipe\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E0D7AE01-1013-4D6E-BE91-FD708C8F6E88}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9CDF7467-C271-444E-AF1D-B12FA281AF3F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-16320" windowWidth="29040" windowHeight="15720" xr2:uid="{A048998D-8A6E-437B-863F-D5E4D7A0533E}"/>
+    <workbookView xWindow="38280" yWindow="5355" windowWidth="38640" windowHeight="15720" xr2:uid="{A048998D-8A6E-437B-863F-D5E4D7A0533E}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="77" uniqueCount="45">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="81" uniqueCount="46">
   <si>
     <t>FICHE DE REVUE DE CODE</t>
   </si>
@@ -314,6 +314,21 @@
         <scheme val="minor"/>
       </rPr>
       <t>(monsieur_tartempion.py)</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Questions No.251 est une question de (*)    "251	 *       Mauvaise  	 Question "  </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>(questions.bd)</t>
     </r>
   </si>
 </sst>
@@ -452,10 +467,10 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -474,7 +489,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Thème Office">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -773,10 +788,10 @@
   <dimension ref="A1:H36"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A10" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="D26" sqref="D26"/>
+      <selection activeCell="K15" sqref="K15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="6" customWidth="1"/>
     <col min="2" max="2" width="14.42578125" customWidth="1"/>
@@ -788,15 +803,15 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A1" s="13" t="s">
+      <c r="A1" s="14" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="13"/>
-      <c r="C1" s="13"/>
-      <c r="D1" s="13"/>
-      <c r="E1" s="13"/>
-      <c r="F1" s="13"/>
-      <c r="G1" s="13"/>
+      <c r="B1" s="14"/>
+      <c r="C1" s="14"/>
+      <c r="D1" s="14"/>
+      <c r="E1" s="14"/>
+      <c r="F1" s="14"/>
+      <c r="G1" s="14"/>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="C3" t="s">
@@ -904,7 +919,7 @@
       <c r="G12" s="12" t="s">
         <v>29</v>
       </c>
-      <c r="H12" s="14"/>
+      <c r="H12" s="13"/>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A13" s="4">
@@ -926,7 +941,7 @@
       <c r="G13" s="12" t="s">
         <v>29</v>
       </c>
-      <c r="H13" s="14"/>
+      <c r="H13" s="13"/>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A14" s="4">
@@ -948,7 +963,7 @@
       <c r="G14" s="12" t="s">
         <v>29</v>
       </c>
-      <c r="H14" s="14"/>
+      <c r="H14" s="13"/>
     </row>
     <row r="15" spans="1:8" ht="39.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="9">
@@ -991,7 +1006,7 @@
       <c r="G16" s="12" t="s">
         <v>29</v>
       </c>
-      <c r="H16" s="14"/>
+      <c r="H16" s="13"/>
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A17" s="4">
@@ -1013,7 +1028,7 @@
       <c r="G17" s="12" t="s">
         <v>29</v>
       </c>
-      <c r="H17" s="14"/>
+      <c r="H17" s="13"/>
     </row>
     <row r="18" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A18" s="4">
@@ -1035,7 +1050,7 @@
       <c r="G18" s="12" t="s">
         <v>29</v>
       </c>
-      <c r="H18" s="14"/>
+      <c r="H18" s="13"/>
     </row>
     <row r="19" spans="1:8" ht="39.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="4">
@@ -1057,7 +1072,7 @@
       <c r="G19" s="12" t="s">
         <v>29</v>
       </c>
-      <c r="H19" s="14"/>
+      <c r="H19" s="13"/>
     </row>
     <row r="20" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A20" s="4">
@@ -1079,7 +1094,7 @@
       <c r="G20" s="12" t="s">
         <v>29</v>
       </c>
-      <c r="H20" s="14"/>
+      <c r="H20" s="13"/>
     </row>
     <row r="21" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A21" s="4">
@@ -1101,7 +1116,7 @@
       <c r="G21" s="12" t="s">
         <v>29</v>
       </c>
-      <c r="H21" s="14"/>
+      <c r="H21" s="13"/>
     </row>
     <row r="22" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A22" s="4">
@@ -1123,7 +1138,7 @@
       <c r="G22" s="12" t="s">
         <v>29</v>
       </c>
-      <c r="H22" s="14"/>
+      <c r="H22" s="13"/>
     </row>
     <row r="23" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A23" s="4">
@@ -1145,18 +1160,29 @@
       <c r="G23" s="12" t="s">
         <v>29</v>
       </c>
-      <c r="H23" s="14"/>
+      <c r="H23" s="13"/>
     </row>
     <row r="24" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A24" s="4">
         <v>13</v>
       </c>
-      <c r="B24" s="4"/>
-      <c r="C24" s="4"/>
-      <c r="D24" s="4"/>
+      <c r="B24" s="4">
+        <v>251</v>
+      </c>
+      <c r="C24" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="D24" s="4" t="s">
+        <v>45</v>
+      </c>
       <c r="E24" s="4"/>
-      <c r="F24" s="4"/>
-      <c r="G24" s="4"/>
+      <c r="F24" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="G24" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="H24" s="13"/>
     </row>
     <row r="25" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A25" s="4">

</xml_diff>

<commit_message>
correction 1 +2 +3 +4 +10 + 14 + 15 (6 moitié)
modification dans le excel ( ajout des erreurs )
</commit_message>
<xml_diff>
--- a/Fichiers equipe/revue_code_Elie.xlsx
+++ b/Fichiers equipe/revue_code_Elie.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lion0203\projets\5GP-Travail_pratique_1\Fichiers equipe\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\efrie\OneDrive - Collège de Bois-de-Boulogne\genie logiciel\Session 5 - Automne 2023\Maintenance logiciel\5GP-Travail_pratique_1\Fichiers equipe\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9CDF7467-C271-444E-AF1D-B12FA281AF3F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D46B6D2F-E324-4282-ADC3-928D4FCF568A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="38280" yWindow="5355" windowWidth="38640" windowHeight="15720" xr2:uid="{A048998D-8A6E-437B-863F-D5E4D7A0533E}"/>
+    <workbookView xWindow="-15" yWindow="-16320" windowWidth="29040" windowHeight="15720" xr2:uid="{A048998D-8A6E-437B-863F-D5E4D7A0533E}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="81" uniqueCount="46">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="85" uniqueCount="47">
   <si>
     <t>FICHE DE REVUE DE CODE</t>
   </si>
@@ -329,6 +329,21 @@
         <scheme val="minor"/>
       </rPr>
       <t>(questions.bd)</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">la paramètre "pardessus: bool" n'est pas necessaire , il est utilisé une seul fois et c'est exactement le même code dans l'autre méthode d'affichage  </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>(monsieur_tartempion.py)</t>
     </r>
   </si>
 </sst>
@@ -489,7 +504,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Thème Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -788,10 +803,10 @@
   <dimension ref="A1:H36"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A10" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="K15" sqref="K15"/>
+      <selection activeCell="D17" sqref="D17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="6" customWidth="1"/>
     <col min="2" max="2" width="14.42578125" customWidth="1"/>
@@ -1184,16 +1199,26 @@
       </c>
       <c r="H24" s="13"/>
     </row>
-    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A25" s="4">
         <v>14</v>
       </c>
-      <c r="B25" s="4"/>
-      <c r="C25" s="4"/>
-      <c r="D25" s="4"/>
+      <c r="B25" s="12">
+        <v>48</v>
+      </c>
+      <c r="C25" s="12" t="s">
+        <v>30</v>
+      </c>
+      <c r="D25" s="7" t="s">
+        <v>46</v>
+      </c>
       <c r="E25" s="4"/>
-      <c r="F25" s="4"/>
-      <c r="G25" s="4"/>
+      <c r="F25" s="12" t="s">
+        <v>7</v>
+      </c>
+      <c r="G25" s="12" t="s">
+        <v>29</v>
+      </c>
     </row>
     <row r="26" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A26" s="4">

</xml_diff>

<commit_message>
Ajouter des taches dans les revue (equipe et Elie)
</commit_message>
<xml_diff>
--- a/Fichiers equipe/revue_code_Elie.xlsx
+++ b/Fichiers equipe/revue_code_Elie.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\efrie\OneDrive - Collège de Bois-de-Boulogne\genie logiciel\Session 5 - Automne 2023\Maintenance logiciel\5GP-Travail_pratique_1\Fichiers equipe\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lion0203\projets\5GP-Travail_pratique_1\Fichiers equipe\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D46B6D2F-E324-4282-ADC3-928D4FCF568A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6434CD6D-30E8-437B-A819-94B72014C1F3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-15" yWindow="-16320" windowWidth="29040" windowHeight="15720" xr2:uid="{A048998D-8A6E-437B-863F-D5E4D7A0533E}"/>
+    <workbookView xWindow="38280" yWindow="-120" windowWidth="38640" windowHeight="15720" xr2:uid="{A048998D-8A6E-437B-863F-D5E4D7A0533E}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="85" uniqueCount="47">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="90" uniqueCount="50">
   <si>
     <t>FICHE DE REVUE DE CODE</t>
   </si>
@@ -334,6 +334,27 @@
   <si>
     <r>
       <t xml:space="preserve">la paramètre "pardessus: bool" n'est pas necessaire , il est utilisé une seul fois et c'est exactement le même code dans l'autre méthode d'affichage  </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>(monsieur_tartempion.py)</t>
+    </r>
+  </si>
+  <si>
+    <t>43 + 48 + 100 +104</t>
+  </si>
+  <si>
+    <t>Défaut + Amélioration</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Duplication du code dans les fonctions , splasher_equipe , splacher_titre, splacher_echec, splasher_succes </t>
     </r>
     <r>
       <rPr>
@@ -391,7 +412,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="6">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -413,12 +434,6 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="0" tint="-0.34998626667073579"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFF00"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -450,25 +465,16 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="14" fontId="0" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -482,10 +488,10 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -504,7 +510,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Thème Office">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -802,14 +808,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{61EF6733-6B20-4ADE-95E8-4F31CB65AA28}">
   <dimension ref="A1:H36"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="D17" sqref="D17"/>
+    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="K9" sqref="K9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="6" customWidth="1"/>
-    <col min="2" max="2" width="14.42578125" customWidth="1"/>
+    <col min="2" max="2" width="18.85546875" customWidth="1"/>
     <col min="3" max="3" width="25.7109375" customWidth="1"/>
     <col min="4" max="4" width="95.7109375" customWidth="1"/>
     <col min="5" max="5" width="17" customWidth="1"/>
@@ -818,15 +824,15 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A1" s="14" t="s">
+      <c r="A1" s="10" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="14"/>
-      <c r="C1" s="14"/>
-      <c r="D1" s="14"/>
-      <c r="E1" s="14"/>
-      <c r="F1" s="14"/>
-      <c r="G1" s="14"/>
+      <c r="B1" s="10"/>
+      <c r="C1" s="10"/>
+      <c r="D1" s="10"/>
+      <c r="E1" s="10"/>
+      <c r="F1" s="10"/>
+      <c r="G1" s="10"/>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="C3" t="s">
@@ -838,7 +844,7 @@
       <c r="E3" t="s">
         <v>2</v>
       </c>
-      <c r="F3" s="6" t="s">
+      <c r="F3" s="5" t="s">
         <v>21</v>
       </c>
     </row>
@@ -852,7 +858,7 @@
       <c r="E4" t="s">
         <v>5</v>
       </c>
-      <c r="F4" s="5">
+      <c r="F4" s="4">
         <v>45204</v>
       </c>
     </row>
@@ -866,7 +872,7 @@
       <c r="E5" t="s">
         <v>8</v>
       </c>
-      <c r="F5" s="5">
+      <c r="F5" s="4">
         <v>45204</v>
       </c>
     </row>
@@ -875,7 +881,7 @@
       <c r="E6" t="s">
         <v>9</v>
       </c>
-      <c r="F6" s="5"/>
+      <c r="F6" s="4"/>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="C7" t="s">
@@ -915,431 +921,445 @@
       </c>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A12" s="4">
+      <c r="A12" s="9">
         <v>1</v>
       </c>
-      <c r="B12" s="11" t="s">
+      <c r="B12" s="8" t="s">
         <v>27</v>
       </c>
-      <c r="C12" s="12" t="s">
+      <c r="C12" s="9" t="s">
         <v>22</v>
       </c>
-      <c r="D12" s="12" t="s">
+      <c r="D12" s="9" t="s">
         <v>32</v>
       </c>
-      <c r="E12" s="12"/>
-      <c r="F12" s="12" t="s">
-        <v>7</v>
-      </c>
-      <c r="G12" s="12" t="s">
-        <v>29</v>
-      </c>
-      <c r="H12" s="13"/>
+      <c r="E12" s="9"/>
+      <c r="F12" s="9" t="s">
+        <v>7</v>
+      </c>
+      <c r="G12" s="9" t="s">
+        <v>29</v>
+      </c>
+      <c r="H12" s="11"/>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A13" s="4">
+      <c r="A13" s="9">
         <v>2</v>
       </c>
-      <c r="B13" s="12" t="s">
+      <c r="B13" s="9" t="s">
         <v>24</v>
       </c>
-      <c r="C13" s="12" t="s">
+      <c r="C13" s="9" t="s">
         <v>23</v>
       </c>
-      <c r="D13" s="9" t="s">
+      <c r="D13" s="6" t="s">
         <v>42</v>
       </c>
-      <c r="E13" s="12"/>
-      <c r="F13" s="12" t="s">
-        <v>7</v>
-      </c>
-      <c r="G13" s="12" t="s">
-        <v>29</v>
-      </c>
-      <c r="H13" s="13"/>
+      <c r="E13" s="9"/>
+      <c r="F13" s="9" t="s">
+        <v>7</v>
+      </c>
+      <c r="G13" s="9" t="s">
+        <v>29</v>
+      </c>
+      <c r="H13" s="11"/>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A14" s="4">
+      <c r="A14" s="9">
         <v>3</v>
       </c>
-      <c r="B14" s="12">
+      <c r="B14" s="9">
         <v>205</v>
       </c>
-      <c r="C14" s="12" t="s">
+      <c r="C14" s="9" t="s">
         <v>25</v>
       </c>
-      <c r="D14" s="9" t="s">
+      <c r="D14" s="6" t="s">
         <v>33</v>
       </c>
-      <c r="E14" s="12"/>
-      <c r="F14" s="12" t="s">
-        <v>7</v>
-      </c>
-      <c r="G14" s="12" t="s">
-        <v>29</v>
-      </c>
-      <c r="H14" s="13"/>
+      <c r="E14" s="9"/>
+      <c r="F14" s="9" t="s">
+        <v>7</v>
+      </c>
+      <c r="G14" s="9" t="s">
+        <v>29</v>
+      </c>
+      <c r="H14" s="11"/>
     </row>
     <row r="15" spans="1:8" ht="39.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="9">
+      <c r="A15" s="6">
         <v>4</v>
       </c>
-      <c r="B15" s="10" t="s">
+      <c r="B15" s="7" t="s">
         <v>27</v>
       </c>
-      <c r="C15" s="9" t="s">
+      <c r="C15" s="6" t="s">
         <v>26</v>
       </c>
-      <c r="D15" s="9" t="s">
+      <c r="D15" s="6" t="s">
         <v>44</v>
       </c>
-      <c r="E15" s="9"/>
-      <c r="F15" s="9" t="s">
-        <v>7</v>
-      </c>
-      <c r="G15" s="9" t="s">
-        <v>29</v>
-      </c>
+      <c r="E15" s="6"/>
+      <c r="F15" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="G15" s="6" t="s">
+        <v>29</v>
+      </c>
+      <c r="H15" s="11"/>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A16" s="4">
+      <c r="A16" s="9">
         <v>5</v>
       </c>
-      <c r="B16" s="12" t="s">
+      <c r="B16" s="9" t="s">
         <v>28</v>
       </c>
-      <c r="C16" s="12" t="s">
+      <c r="C16" s="9" t="s">
         <v>26</v>
       </c>
-      <c r="D16" s="9" t="s">
+      <c r="D16" s="6" t="s">
         <v>34</v>
       </c>
-      <c r="E16" s="12"/>
-      <c r="F16" s="12" t="s">
-        <v>7</v>
-      </c>
-      <c r="G16" s="12" t="s">
-        <v>29</v>
-      </c>
-      <c r="H16" s="13"/>
+      <c r="E16" s="9"/>
+      <c r="F16" s="9" t="s">
+        <v>7</v>
+      </c>
+      <c r="G16" s="9" t="s">
+        <v>29</v>
+      </c>
+      <c r="H16" s="11"/>
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A17" s="4">
+      <c r="A17" s="9">
         <v>6</v>
       </c>
-      <c r="B17" s="12">
+      <c r="B17" s="9">
         <v>128</v>
       </c>
-      <c r="C17" s="12" t="s">
+      <c r="C17" s="9" t="s">
         <v>31</v>
       </c>
-      <c r="D17" s="9" t="s">
+      <c r="D17" s="6" t="s">
         <v>35</v>
       </c>
-      <c r="E17" s="12"/>
-      <c r="F17" s="12" t="s">
-        <v>7</v>
-      </c>
-      <c r="G17" s="12" t="s">
-        <v>29</v>
-      </c>
-      <c r="H17" s="13"/>
+      <c r="E17" s="9"/>
+      <c r="F17" s="9" t="s">
+        <v>7</v>
+      </c>
+      <c r="G17" s="9" t="s">
+        <v>29</v>
+      </c>
+      <c r="H17" s="11"/>
     </row>
     <row r="18" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A18" s="4">
-        <v>7</v>
-      </c>
-      <c r="B18" s="12">
+      <c r="A18" s="9">
+        <v>7</v>
+      </c>
+      <c r="B18" s="9">
         <v>45</v>
       </c>
-      <c r="C18" s="12" t="s">
+      <c r="C18" s="9" t="s">
         <v>23</v>
       </c>
-      <c r="D18" s="9" t="s">
+      <c r="D18" s="6" t="s">
         <v>36</v>
       </c>
-      <c r="E18" s="12"/>
-      <c r="F18" s="12" t="s">
-        <v>7</v>
-      </c>
-      <c r="G18" s="12" t="s">
-        <v>29</v>
-      </c>
-      <c r="H18" s="13"/>
+      <c r="E18" s="9"/>
+      <c r="F18" s="9" t="s">
+        <v>7</v>
+      </c>
+      <c r="G18" s="9" t="s">
+        <v>29</v>
+      </c>
+      <c r="H18" s="11"/>
     </row>
     <row r="19" spans="1:8" ht="39.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="4">
+      <c r="A19" s="9">
         <v>8</v>
       </c>
-      <c r="B19" s="11" t="s">
+      <c r="B19" s="8" t="s">
         <v>27</v>
       </c>
-      <c r="C19" s="12" t="s">
+      <c r="C19" s="9" t="s">
         <v>30</v>
       </c>
-      <c r="D19" s="12" t="s">
+      <c r="D19" s="9" t="s">
         <v>39</v>
       </c>
-      <c r="E19" s="12"/>
-      <c r="F19" s="12" t="s">
-        <v>7</v>
-      </c>
-      <c r="G19" s="12" t="s">
-        <v>29</v>
-      </c>
-      <c r="H19" s="13"/>
+      <c r="E19" s="9"/>
+      <c r="F19" s="9" t="s">
+        <v>7</v>
+      </c>
+      <c r="G19" s="9" t="s">
+        <v>29</v>
+      </c>
+      <c r="H19" s="11"/>
     </row>
     <row r="20" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A20" s="4">
+      <c r="A20" s="9">
         <v>9</v>
       </c>
-      <c r="B20" s="12">
+      <c r="B20" s="9">
         <v>241</v>
       </c>
-      <c r="C20" s="12" t="s">
+      <c r="C20" s="9" t="s">
         <v>22</v>
       </c>
-      <c r="D20" s="12" t="s">
+      <c r="D20" s="9" t="s">
         <v>37</v>
       </c>
-      <c r="E20" s="12"/>
-      <c r="F20" s="12" t="s">
-        <v>7</v>
-      </c>
-      <c r="G20" s="12" t="s">
-        <v>29</v>
-      </c>
-      <c r="H20" s="13"/>
+      <c r="E20" s="9"/>
+      <c r="F20" s="9" t="s">
+        <v>7</v>
+      </c>
+      <c r="G20" s="9" t="s">
+        <v>29</v>
+      </c>
+      <c r="H20" s="11"/>
     </row>
     <row r="21" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A21" s="4">
+      <c r="A21" s="9">
         <v>10</v>
       </c>
-      <c r="B21" s="11" t="s">
+      <c r="B21" s="8" t="s">
         <v>27</v>
       </c>
-      <c r="C21" s="12" t="s">
+      <c r="C21" s="9" t="s">
         <v>31</v>
       </c>
-      <c r="D21" s="9" t="s">
+      <c r="D21" s="6" t="s">
         <v>38</v>
       </c>
-      <c r="E21" s="12"/>
-      <c r="F21" s="12" t="s">
-        <v>7</v>
-      </c>
-      <c r="G21" s="12" t="s">
-        <v>29</v>
-      </c>
-      <c r="H21" s="13"/>
+      <c r="E21" s="9"/>
+      <c r="F21" s="9" t="s">
+        <v>7</v>
+      </c>
+      <c r="G21" s="9" t="s">
+        <v>29</v>
+      </c>
+      <c r="H21" s="11"/>
     </row>
     <row r="22" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A22" s="4">
+      <c r="A22" s="9">
         <v>11</v>
       </c>
       <c r="B22" s="8" t="s">
         <v>27</v>
       </c>
-      <c r="C22" s="4" t="s">
+      <c r="C22" s="9" t="s">
         <v>26</v>
       </c>
-      <c r="D22" s="7" t="s">
+      <c r="D22" s="6" t="s">
         <v>40</v>
       </c>
-      <c r="E22" s="4"/>
-      <c r="F22" s="12" t="s">
-        <v>7</v>
-      </c>
-      <c r="G22" s="12" t="s">
-        <v>29</v>
-      </c>
-      <c r="H22" s="13"/>
+      <c r="E22" s="9"/>
+      <c r="F22" s="9" t="s">
+        <v>7</v>
+      </c>
+      <c r="G22" s="9" t="s">
+        <v>29</v>
+      </c>
+      <c r="H22" s="11"/>
     </row>
     <row r="23" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A23" s="4">
+      <c r="A23" s="9">
         <v>12</v>
       </c>
-      <c r="B23" s="4">
+      <c r="B23" s="9">
         <v>162</v>
       </c>
-      <c r="C23" s="4" t="s">
+      <c r="C23" s="9" t="s">
         <v>41</v>
       </c>
-      <c r="D23" s="7" t="s">
+      <c r="D23" s="6" t="s">
         <v>43</v>
       </c>
-      <c r="E23" s="4"/>
-      <c r="F23" s="12" t="s">
-        <v>7</v>
-      </c>
-      <c r="G23" s="12" t="s">
-        <v>29</v>
-      </c>
-      <c r="H23" s="13"/>
+      <c r="E23" s="9"/>
+      <c r="F23" s="9" t="s">
+        <v>7</v>
+      </c>
+      <c r="G23" s="9" t="s">
+        <v>29</v>
+      </c>
+      <c r="H23" s="11"/>
     </row>
     <row r="24" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A24" s="4">
+      <c r="A24" s="9">
         <v>13</v>
       </c>
-      <c r="B24" s="4">
+      <c r="B24" s="9">
         <v>251</v>
       </c>
-      <c r="C24" s="4" t="s">
+      <c r="C24" s="9" t="s">
         <v>31</v>
       </c>
-      <c r="D24" s="4" t="s">
+      <c r="D24" s="9" t="s">
         <v>45</v>
       </c>
-      <c r="E24" s="4"/>
-      <c r="F24" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="G24" s="4" t="s">
-        <v>29</v>
-      </c>
-      <c r="H24" s="13"/>
+      <c r="E24" s="9"/>
+      <c r="F24" s="9" t="s">
+        <v>7</v>
+      </c>
+      <c r="G24" s="9" t="s">
+        <v>29</v>
+      </c>
+      <c r="H24" s="11"/>
     </row>
     <row r="25" spans="1:8" ht="30" x14ac:dyDescent="0.25">
-      <c r="A25" s="4">
+      <c r="A25" s="9">
         <v>14</v>
       </c>
-      <c r="B25" s="12">
+      <c r="B25" s="9">
         <v>48</v>
       </c>
-      <c r="C25" s="12" t="s">
+      <c r="C25" s="9" t="s">
         <v>30</v>
       </c>
-      <c r="D25" s="7" t="s">
+      <c r="D25" s="6" t="s">
         <v>46</v>
       </c>
-      <c r="E25" s="4"/>
-      <c r="F25" s="12" t="s">
-        <v>7</v>
-      </c>
-      <c r="G25" s="12" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A26" s="4">
+      <c r="E25" s="9"/>
+      <c r="F25" s="9" t="s">
+        <v>7</v>
+      </c>
+      <c r="G25" s="9" t="s">
+        <v>29</v>
+      </c>
+      <c r="H25" s="11"/>
+    </row>
+    <row r="26" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+      <c r="A26" s="9">
         <v>15</v>
       </c>
-      <c r="B26" s="4"/>
-      <c r="C26" s="4"/>
-      <c r="D26" s="4"/>
-      <c r="E26" s="4"/>
-      <c r="F26" s="4"/>
-      <c r="G26" s="4"/>
+      <c r="B26" s="9" t="s">
+        <v>47</v>
+      </c>
+      <c r="C26" s="9" t="s">
+        <v>48</v>
+      </c>
+      <c r="D26" s="6" t="s">
+        <v>49</v>
+      </c>
+      <c r="E26" s="9"/>
+      <c r="F26" s="9" t="s">
+        <v>7</v>
+      </c>
+      <c r="G26" s="9" t="s">
+        <v>29</v>
+      </c>
+      <c r="H26" s="11"/>
     </row>
     <row r="27" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A27" s="4">
+      <c r="A27" s="9">
         <v>16</v>
       </c>
-      <c r="B27" s="4"/>
-      <c r="C27" s="4"/>
-      <c r="D27" s="4"/>
-      <c r="E27" s="4"/>
-      <c r="F27" s="4"/>
-      <c r="G27" s="4"/>
+      <c r="B27" s="9"/>
+      <c r="C27" s="9"/>
+      <c r="D27" s="9"/>
+      <c r="E27" s="9"/>
+      <c r="F27" s="9"/>
+      <c r="G27" s="9"/>
+      <c r="H27" s="11"/>
     </row>
     <row r="28" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A28" s="4">
+      <c r="A28" s="9">
         <v>17</v>
       </c>
-      <c r="B28" s="4"/>
-      <c r="C28" s="4"/>
-      <c r="D28" s="4"/>
-      <c r="E28" s="4"/>
-      <c r="F28" s="4"/>
-      <c r="G28" s="4"/>
+      <c r="B28" s="9"/>
+      <c r="C28" s="9"/>
+      <c r="D28" s="9"/>
+      <c r="E28" s="9"/>
+      <c r="F28" s="9"/>
+      <c r="G28" s="9"/>
     </row>
     <row r="29" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A29" s="4">
+      <c r="A29" s="9">
         <v>18</v>
       </c>
-      <c r="B29" s="4"/>
-      <c r="C29" s="4"/>
-      <c r="D29" s="4"/>
-      <c r="E29" s="4"/>
-      <c r="F29" s="4"/>
-      <c r="G29" s="4"/>
+      <c r="B29" s="9"/>
+      <c r="C29" s="9"/>
+      <c r="D29" s="9"/>
+      <c r="E29" s="9"/>
+      <c r="F29" s="9"/>
+      <c r="G29" s="9"/>
     </row>
     <row r="30" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A30" s="4">
+      <c r="A30" s="9">
         <v>19</v>
       </c>
-      <c r="B30" s="4"/>
-      <c r="C30" s="4"/>
-      <c r="D30" s="4"/>
-      <c r="E30" s="4"/>
-      <c r="F30" s="4"/>
-      <c r="G30" s="4"/>
+      <c r="B30" s="9"/>
+      <c r="C30" s="9"/>
+      <c r="D30" s="9"/>
+      <c r="E30" s="9"/>
+      <c r="F30" s="9"/>
+      <c r="G30" s="9"/>
     </row>
     <row r="31" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A31" s="4">
+      <c r="A31" s="9">
         <v>20</v>
       </c>
-      <c r="B31" s="4"/>
-      <c r="C31" s="4"/>
-      <c r="D31" s="4"/>
-      <c r="E31" s="4"/>
-      <c r="F31" s="4"/>
-      <c r="G31" s="4"/>
+      <c r="B31" s="9"/>
+      <c r="C31" s="9"/>
+      <c r="D31" s="9"/>
+      <c r="E31" s="9"/>
+      <c r="F31" s="9"/>
+      <c r="G31" s="9"/>
     </row>
     <row r="32" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A32" s="4">
+      <c r="A32" s="9">
         <v>21</v>
       </c>
-      <c r="B32" s="4"/>
-      <c r="C32" s="4"/>
-      <c r="D32" s="4"/>
-      <c r="E32" s="4"/>
-      <c r="F32" s="4"/>
-      <c r="G32" s="4"/>
+      <c r="B32" s="9"/>
+      <c r="C32" s="9"/>
+      <c r="D32" s="9"/>
+      <c r="E32" s="9"/>
+      <c r="F32" s="9"/>
+      <c r="G32" s="9"/>
     </row>
     <row r="33" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A33" s="4">
+      <c r="A33" s="9">
         <v>22</v>
       </c>
-      <c r="B33" s="4"/>
-      <c r="C33" s="4"/>
-      <c r="D33" s="4"/>
-      <c r="E33" s="4"/>
-      <c r="F33" s="4"/>
-      <c r="G33" s="4"/>
+      <c r="B33" s="9"/>
+      <c r="C33" s="9"/>
+      <c r="D33" s="9"/>
+      <c r="E33" s="9"/>
+      <c r="F33" s="9"/>
+      <c r="G33" s="9"/>
     </row>
     <row r="34" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A34" s="4">
+      <c r="A34" s="9">
         <v>23</v>
       </c>
-      <c r="B34" s="4"/>
-      <c r="C34" s="4"/>
-      <c r="D34" s="4"/>
-      <c r="E34" s="4"/>
-      <c r="F34" s="4"/>
-      <c r="G34" s="4"/>
+      <c r="B34" s="9"/>
+      <c r="C34" s="9"/>
+      <c r="D34" s="9"/>
+      <c r="E34" s="9"/>
+      <c r="F34" s="9"/>
+      <c r="G34" s="9"/>
     </row>
     <row r="35" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A35" s="4">
+      <c r="A35" s="9">
         <v>24</v>
       </c>
-      <c r="B35" s="4"/>
-      <c r="C35" s="4"/>
-      <c r="D35" s="4"/>
-      <c r="E35" s="4"/>
-      <c r="F35" s="4"/>
-      <c r="G35" s="4"/>
+      <c r="B35" s="9"/>
+      <c r="C35" s="9"/>
+      <c r="D35" s="9"/>
+      <c r="E35" s="9"/>
+      <c r="F35" s="9"/>
+      <c r="G35" s="9"/>
     </row>
     <row r="36" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A36" s="4">
+      <c r="A36" s="9">
         <v>25</v>
       </c>
-      <c r="B36" s="4"/>
-      <c r="C36" s="4"/>
-      <c r="D36" s="4"/>
-      <c r="E36" s="4"/>
-      <c r="F36" s="4"/>
-      <c r="G36" s="4"/>
+      <c r="B36" s="9"/>
+      <c r="C36" s="9"/>
+      <c r="D36" s="9"/>
+      <c r="E36" s="9"/>
+      <c r="F36" s="9"/>
+      <c r="G36" s="9"/>
     </row>
   </sheetData>
   <mergeCells count="1">

</xml_diff>

<commit_message>
Correction erreurs + changement document revue equipe
</commit_message>
<xml_diff>
--- a/Fichiers equipe/revue_code_Elie.xlsx
+++ b/Fichiers equipe/revue_code_Elie.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26626"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26731"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lion0203\projets\5GP-Travail_pratique_1\Fichiers equipe\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\dinaa\Documents\Maintenace Logiciel\5GP-Travail_pratique_1\Fichiers equipe\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6434CD6D-30E8-437B-A819-94B72014C1F3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8C2A464E-044D-47A1-B8B9-8A7F46A212C7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="38280" yWindow="-120" windowWidth="38640" windowHeight="15720" xr2:uid="{A048998D-8A6E-437B-863F-D5E4D7A0533E}"/>
+    <workbookView xWindow="-104" yWindow="-104" windowWidth="22326" windowHeight="11947" xr2:uid="{A048998D-8A6E-437B-863F-D5E4D7A0533E}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -465,7 +465,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
@@ -491,7 +491,6 @@
     <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -806,24 +805,24 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{61EF6733-6B20-4ADE-95E8-4F31CB65AA28}">
-  <dimension ref="A1:H36"/>
+  <dimension ref="A1:G36"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="K9" sqref="K9"/>
+    <sheetView tabSelected="1" topLeftCell="A7" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="H15" sqref="H15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.09765625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="6" customWidth="1"/>
-    <col min="2" max="2" width="18.85546875" customWidth="1"/>
-    <col min="3" max="3" width="25.7109375" customWidth="1"/>
-    <col min="4" max="4" width="95.7109375" customWidth="1"/>
+    <col min="2" max="2" width="18.8984375" customWidth="1"/>
+    <col min="3" max="3" width="25.69921875" customWidth="1"/>
+    <col min="4" max="4" width="95.69921875" customWidth="1"/>
     <col min="5" max="5" width="17" customWidth="1"/>
-    <col min="6" max="6" width="20.28515625" customWidth="1"/>
-    <col min="7" max="7" width="14.28515625" customWidth="1"/>
+    <col min="6" max="6" width="20.296875" customWidth="1"/>
+    <col min="7" max="7" width="14.296875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:7" ht="17.850000000000001" x14ac:dyDescent="0.35">
       <c r="A1" s="10" t="s">
         <v>0</v>
       </c>
@@ -834,7 +833,7 @@
       <c r="F1" s="10"/>
       <c r="G1" s="10"/>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
       <c r="C3" t="s">
         <v>1</v>
       </c>
@@ -848,7 +847,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
       <c r="C4" t="s">
         <v>3</v>
       </c>
@@ -862,7 +861,7 @@
         <v>45204</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
       <c r="C5" t="s">
         <v>6</v>
       </c>
@@ -876,20 +875,20 @@
         <v>45204</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
       <c r="D6" s="2"/>
       <c r="E6" t="s">
         <v>9</v>
       </c>
       <c r="F6" s="4"/>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
       <c r="C7" t="s">
         <v>10</v>
       </c>
       <c r="D7" s="2"/>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
       <c r="C9" s="1" t="s">
         <v>11</v>
       </c>
@@ -897,7 +896,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A11" s="3" t="s">
         <v>13</v>
       </c>
@@ -920,7 +919,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A12" s="9">
         <v>1</v>
       </c>
@@ -940,9 +939,8 @@
       <c r="G12" s="9" t="s">
         <v>29</v>
       </c>
-      <c r="H12" s="11"/>
-    </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A13" s="9">
         <v>2</v>
       </c>
@@ -962,9 +960,8 @@
       <c r="G13" s="9" t="s">
         <v>29</v>
       </c>
-      <c r="H13" s="11"/>
-    </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A14" s="9">
         <v>3</v>
       </c>
@@ -984,9 +981,8 @@
       <c r="G14" s="9" t="s">
         <v>29</v>
       </c>
-      <c r="H14" s="11"/>
-    </row>
-    <row r="15" spans="1:8" ht="39.75" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="15" spans="1:7" ht="39.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A15" s="6">
         <v>4</v>
       </c>
@@ -1006,9 +1002,8 @@
       <c r="G15" s="6" t="s">
         <v>29</v>
       </c>
-      <c r="H15" s="11"/>
-    </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A16" s="9">
         <v>5</v>
       </c>
@@ -1028,9 +1023,8 @@
       <c r="G16" s="9" t="s">
         <v>29</v>
       </c>
-      <c r="H16" s="11"/>
-    </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A17" s="9">
         <v>6</v>
       </c>
@@ -1050,9 +1044,8 @@
       <c r="G17" s="9" t="s">
         <v>29</v>
       </c>
-      <c r="H17" s="11"/>
-    </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A18" s="9">
         <v>7</v>
       </c>
@@ -1072,9 +1065,8 @@
       <c r="G18" s="9" t="s">
         <v>29</v>
       </c>
-      <c r="H18" s="11"/>
-    </row>
-    <row r="19" spans="1:8" ht="39.75" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="19" spans="1:7" ht="39.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A19" s="9">
         <v>8</v>
       </c>
@@ -1094,9 +1086,8 @@
       <c r="G19" s="9" t="s">
         <v>29</v>
       </c>
-      <c r="H19" s="11"/>
-    </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A20" s="9">
         <v>9</v>
       </c>
@@ -1116,9 +1107,8 @@
       <c r="G20" s="9" t="s">
         <v>29</v>
       </c>
-      <c r="H20" s="11"/>
-    </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A21" s="9">
         <v>10</v>
       </c>
@@ -1138,9 +1128,8 @@
       <c r="G21" s="9" t="s">
         <v>29</v>
       </c>
-      <c r="H21" s="11"/>
-    </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
+    </row>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A22" s="9">
         <v>11</v>
       </c>
@@ -1160,9 +1149,8 @@
       <c r="G22" s="9" t="s">
         <v>29</v>
       </c>
-      <c r="H22" s="11"/>
-    </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
+    </row>
+    <row r="23" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A23" s="9">
         <v>12</v>
       </c>
@@ -1182,9 +1170,8 @@
       <c r="G23" s="9" t="s">
         <v>29</v>
       </c>
-      <c r="H23" s="11"/>
-    </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
+    </row>
+    <row r="24" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A24" s="9">
         <v>13</v>
       </c>
@@ -1204,9 +1191,8 @@
       <c r="G24" s="9" t="s">
         <v>29</v>
       </c>
-      <c r="H24" s="11"/>
-    </row>
-    <row r="25" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+    </row>
+    <row r="25" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A25" s="9">
         <v>14</v>
       </c>
@@ -1226,9 +1212,8 @@
       <c r="G25" s="9" t="s">
         <v>29</v>
       </c>
-      <c r="H25" s="11"/>
-    </row>
-    <row r="26" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+    </row>
+    <row r="26" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A26" s="9">
         <v>15</v>
       </c>
@@ -1248,9 +1233,8 @@
       <c r="G26" s="9" t="s">
         <v>29</v>
       </c>
-      <c r="H26" s="11"/>
-    </row>
-    <row r="27" spans="1:8" x14ac:dyDescent="0.25">
+    </row>
+    <row r="27" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A27" s="9">
         <v>16</v>
       </c>
@@ -1260,9 +1244,8 @@
       <c r="E27" s="9"/>
       <c r="F27" s="9"/>
       <c r="G27" s="9"/>
-      <c r="H27" s="11"/>
-    </row>
-    <row r="28" spans="1:8" x14ac:dyDescent="0.25">
+    </row>
+    <row r="28" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A28" s="9">
         <v>17</v>
       </c>
@@ -1273,7 +1256,7 @@
       <c r="F28" s="9"/>
       <c r="G28" s="9"/>
     </row>
-    <row r="29" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A29" s="9">
         <v>18</v>
       </c>
@@ -1284,7 +1267,7 @@
       <c r="F29" s="9"/>
       <c r="G29" s="9"/>
     </row>
-    <row r="30" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A30" s="9">
         <v>19</v>
       </c>
@@ -1295,7 +1278,7 @@
       <c r="F30" s="9"/>
       <c r="G30" s="9"/>
     </row>
-    <row r="31" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A31" s="9">
         <v>20</v>
       </c>
@@ -1306,7 +1289,7 @@
       <c r="F31" s="9"/>
       <c r="G31" s="9"/>
     </row>
-    <row r="32" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A32" s="9">
         <v>21</v>
       </c>
@@ -1317,7 +1300,7 @@
       <c r="F32" s="9"/>
       <c r="G32" s="9"/>
     </row>
-    <row r="33" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A33" s="9">
         <v>22</v>
       </c>
@@ -1328,7 +1311,7 @@
       <c r="F33" s="9"/>
       <c r="G33" s="9"/>
     </row>
-    <row r="34" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A34" s="9">
         <v>23</v>
       </c>
@@ -1339,7 +1322,7 @@
       <c r="F34" s="9"/>
       <c r="G34" s="9"/>
     </row>
-    <row r="35" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A35" s="9">
         <v>24</v>
       </c>
@@ -1350,7 +1333,7 @@
       <c r="F35" s="9"/>
       <c r="G35" s="9"/>
     </row>
-    <row r="36" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A36" s="9">
         <v>25</v>
       </c>

</xml_diff>

<commit_message>
modification du temps pour une nouvelle partie , changement dans la revue
</commit_message>
<xml_diff>
--- a/Fichiers equipe/revue_code_Elie.xlsx
+++ b/Fichiers equipe/revue_code_Elie.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\dinaa\Documents\Maintenace Logiciel\5GP-Travail_pratique_1\Fichiers equipe\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lion0203\projets\5GP-Travail_pratique_1\Fichiers equipe\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8C2A464E-044D-47A1-B8B9-8A7F46A212C7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C10E425E-3642-4395-A0A0-48EB44DDC536}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-104" yWindow="-104" windowWidth="22326" windowHeight="11947" xr2:uid="{A048998D-8A6E-437B-863F-D5E4D7A0533E}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" xr2:uid="{A048998D-8A6E-437B-863F-D5E4D7A0533E}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="90" uniqueCount="50">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="99" uniqueCount="53">
   <si>
     <t>FICHE DE REVUE DE CODE</t>
   </si>
@@ -365,6 +365,39 @@
         <scheme val="minor"/>
       </rPr>
       <t>(monsieur_tartempion.py)</t>
+    </r>
+  </si>
+  <si>
+    <t>187 + 212</t>
+  </si>
+  <si>
+    <r>
+      <t>Des commentaires mal placés qui décrivent la fonctionnalité du programme dans des endroits inappropriés</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>.(monsieur_tartempion.py)</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">À la fin du partie , le temps ne revennait pas a 60 en commencant une nouvelle partie </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> (monsieur_tartempion.py)</t>
     </r>
   </si>
 </sst>
@@ -807,22 +840,22 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{61EF6733-6B20-4ADE-95E8-4F31CB65AA28}">
   <dimension ref="A1:G36"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="H15" sqref="H15"/>
+    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="K25" sqref="K25"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.09765625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="6" customWidth="1"/>
-    <col min="2" max="2" width="18.8984375" customWidth="1"/>
-    <col min="3" max="3" width="25.69921875" customWidth="1"/>
-    <col min="4" max="4" width="95.69921875" customWidth="1"/>
+    <col min="2" max="2" width="18.85546875" customWidth="1"/>
+    <col min="3" max="3" width="25.7109375" customWidth="1"/>
+    <col min="4" max="4" width="95.7109375" customWidth="1"/>
     <col min="5" max="5" width="17" customWidth="1"/>
-    <col min="6" max="6" width="20.296875" customWidth="1"/>
-    <col min="7" max="7" width="14.296875" customWidth="1"/>
+    <col min="6" max="6" width="20.28515625" customWidth="1"/>
+    <col min="7" max="7" width="14.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="17.850000000000001" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:7" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A1" s="10" t="s">
         <v>0</v>
       </c>
@@ -833,7 +866,7 @@
       <c r="F1" s="10"/>
       <c r="G1" s="10"/>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="C3" t="s">
         <v>1</v>
       </c>
@@ -847,7 +880,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="C4" t="s">
         <v>3</v>
       </c>
@@ -861,7 +894,7 @@
         <v>45204</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="C5" t="s">
         <v>6</v>
       </c>
@@ -875,20 +908,20 @@
         <v>45204</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="D6" s="2"/>
       <c r="E6" t="s">
         <v>9</v>
       </c>
       <c r="F6" s="4"/>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="C7" t="s">
         <v>10</v>
       </c>
       <c r="D7" s="2"/>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="C9" s="1" t="s">
         <v>11</v>
       </c>
@@ -896,7 +929,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11" s="3" t="s">
         <v>13</v>
       </c>
@@ -919,7 +952,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A12" s="9">
         <v>1</v>
       </c>
@@ -940,7 +973,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A13" s="9">
         <v>2</v>
       </c>
@@ -961,7 +994,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A14" s="9">
         <v>3</v>
       </c>
@@ -982,7 +1015,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="15" spans="1:7" ht="39.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:7" ht="39.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="6">
         <v>4</v>
       </c>
@@ -1003,7 +1036,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A16" s="9">
         <v>5</v>
       </c>
@@ -1024,7 +1057,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A17" s="9">
         <v>6</v>
       </c>
@@ -1045,7 +1078,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A18" s="9">
         <v>7</v>
       </c>
@@ -1066,7 +1099,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="19" spans="1:7" ht="39.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:7" ht="39.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="9">
         <v>8</v>
       </c>
@@ -1076,7 +1109,7 @@
       <c r="C19" s="9" t="s">
         <v>30</v>
       </c>
-      <c r="D19" s="9" t="s">
+      <c r="D19" s="6" t="s">
         <v>39</v>
       </c>
       <c r="E19" s="9"/>
@@ -1087,7 +1120,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A20" s="9">
         <v>9</v>
       </c>
@@ -1108,7 +1141,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A21" s="9">
         <v>10</v>
       </c>
@@ -1129,7 +1162,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A22" s="9">
         <v>11</v>
       </c>
@@ -1150,7 +1183,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A23" s="9">
         <v>12</v>
       </c>
@@ -1171,7 +1204,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A24" s="9">
         <v>13</v>
       </c>
@@ -1192,7 +1225,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="25" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A25" s="9">
         <v>14</v>
       </c>
@@ -1213,7 +1246,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="26" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A26" s="9">
         <v>15</v>
       </c>
@@ -1234,29 +1267,49 @@
         <v>29</v>
       </c>
     </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A27" s="9">
         <v>16</v>
       </c>
-      <c r="B27" s="9"/>
-      <c r="C27" s="9"/>
-      <c r="D27" s="9"/>
+      <c r="B27" s="9" t="s">
+        <v>50</v>
+      </c>
+      <c r="C27" s="9" t="s">
+        <v>31</v>
+      </c>
+      <c r="D27" s="6" t="s">
+        <v>51</v>
+      </c>
       <c r="E27" s="9"/>
-      <c r="F27" s="9"/>
-      <c r="G27" s="9"/>
-    </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="F27" s="9" t="s">
+        <v>7</v>
+      </c>
+      <c r="G27" s="9" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="28" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A28" s="9">
         <v>17</v>
       </c>
-      <c r="B28" s="9"/>
-      <c r="C28" s="9"/>
-      <c r="D28" s="9"/>
+      <c r="B28" s="9">
+        <v>205</v>
+      </c>
+      <c r="C28" s="9" t="s">
+        <v>31</v>
+      </c>
+      <c r="D28" s="6" t="s">
+        <v>52</v>
+      </c>
       <c r="E28" s="9"/>
-      <c r="F28" s="9"/>
-      <c r="G28" s="9"/>
-    </row>
-    <row r="29" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="F28" s="9" t="s">
+        <v>7</v>
+      </c>
+      <c r="G28" s="9" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A29" s="9">
         <v>18</v>
       </c>
@@ -1267,7 +1320,7 @@
       <c r="F29" s="9"/>
       <c r="G29" s="9"/>
     </row>
-    <row r="30" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A30" s="9">
         <v>19</v>
       </c>
@@ -1278,7 +1331,7 @@
       <c r="F30" s="9"/>
       <c r="G30" s="9"/>
     </row>
-    <row r="31" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A31" s="9">
         <v>20</v>
       </c>
@@ -1289,7 +1342,7 @@
       <c r="F31" s="9"/>
       <c r="G31" s="9"/>
     </row>
-    <row r="32" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A32" s="9">
         <v>21</v>
       </c>
@@ -1300,7 +1353,7 @@
       <c r="F32" s="9"/>
       <c r="G32" s="9"/>
     </row>
-    <row r="33" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A33" s="9">
         <v>22</v>
       </c>
@@ -1311,7 +1364,7 @@
       <c r="F33" s="9"/>
       <c r="G33" s="9"/>
     </row>
-    <row r="34" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A34" s="9">
         <v>23</v>
       </c>
@@ -1322,7 +1375,7 @@
       <c r="F34" s="9"/>
       <c r="G34" s="9"/>
     </row>
-    <row r="35" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A35" s="9">
         <v>24</v>
       </c>
@@ -1333,7 +1386,7 @@
       <c r="F35" s="9"/>
       <c r="G35" s="9"/>
     </row>
-    <row r="36" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A36" s="9">
         <v>25</v>
       </c>

</xml_diff>